<commit_message>
chore: add dummy data
</commit_message>
<xml_diff>
--- a/src/library_manager/Books.xlsx
+++ b/src/library_manager/Books.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -409,10 +409,21 @@
       <c r="B1" t="str">
         <v>book</v>
       </c>
+      <c r="F1" t="str">
+        <v>quantity</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>book1</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>